<commit_message>
mudanças nos textos e nas taxas de reforma de segundo grau, incorporando informações atualizadas
</commit_message>
<xml_diff>
--- a/inst/da_cposg_tidy.xlsx
+++ b/inst/da_cposg_tidy.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,6 +398,11 @@
           <t>tem_decisao</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -428,6 +433,11 @@
       <c r="H2" t="b">
         <v>1</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -458,6 +468,11 @@
       <c r="H3" t="b">
         <v>1</v>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -498,6 +513,11 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -538,6 +558,11 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -578,6 +603,11 @@
       <c r="H6" t="b">
         <v>1</v>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -618,6 +648,11 @@
       <c r="H7" t="b">
         <v>1</v>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +683,11 @@
       <c r="H8" t="b">
         <v>1</v>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -688,6 +728,11 @@
       <c r="H9" t="b">
         <v>1</v>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -728,6 +773,11 @@
       <c r="H10" t="b">
         <v>1</v>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -768,6 +818,11 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -798,6 +853,11 @@
       <c r="H12" t="b">
         <v>1</v>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -828,6 +888,11 @@
       <c r="H13" t="b">
         <v>1</v>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -868,6 +933,11 @@
       <c r="H14" t="b">
         <v>1</v>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -908,6 +978,11 @@
       <c r="H15" t="b">
         <v>1</v>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -938,6 +1013,11 @@
       <c r="H16" t="b">
         <v>1</v>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -978,6 +1058,11 @@
       <c r="H17" t="b">
         <v>1</v>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1018,6 +1103,11 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1058,6 +1148,11 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1098,6 +1193,11 @@
       <c r="H20" t="b">
         <v>1</v>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1138,6 +1238,11 @@
       <c r="H21" t="b">
         <v>1</v>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1178,6 +1283,11 @@
       <c r="H22" t="b">
         <v>1</v>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1218,6 +1328,11 @@
       <c r="H23" t="b">
         <v>1</v>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1258,6 +1373,11 @@
       <c r="H24" t="b">
         <v>1</v>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1298,6 +1418,11 @@
       <c r="H25" t="b">
         <v>1</v>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1338,6 +1463,11 @@
       <c r="H26" t="b">
         <v>1</v>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1368,6 +1498,11 @@
       <c r="H27" t="b">
         <v>1</v>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1408,6 +1543,11 @@
       <c r="H28" t="b">
         <v>1</v>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1448,6 +1588,11 @@
       <c r="H29" t="b">
         <v>1</v>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1488,6 +1633,11 @@
       <c r="H30" t="b">
         <v>1</v>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1528,6 +1678,11 @@
       <c r="H31" t="b">
         <v>1</v>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1558,6 +1713,11 @@
       <c r="H32" t="b">
         <v>1</v>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1598,6 +1758,11 @@
       <c r="H33" t="b">
         <v>1</v>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1628,6 +1793,11 @@
       <c r="H34" t="b">
         <v>1</v>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1668,6 +1838,11 @@
       <c r="H35" t="b">
         <v>1</v>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1708,6 +1883,11 @@
       <c r="H36" t="b">
         <v>1</v>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1738,6 +1918,11 @@
       <c r="H37" t="b">
         <v>1</v>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1778,6 +1963,11 @@
       <c r="H38" t="b">
         <v>1</v>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1818,6 +2008,11 @@
       <c r="H39" t="b">
         <v>1</v>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1858,6 +2053,11 @@
       <c r="H40" t="b">
         <v>1</v>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1898,6 +2098,11 @@
       <c r="H41" t="b">
         <v>1</v>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1938,6 +2143,11 @@
       <c r="H42" t="b">
         <v>1</v>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1978,6 +2188,11 @@
       <c r="H43" t="b">
         <v>1</v>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2018,6 +2233,11 @@
       <c r="H44" t="b">
         <v>1</v>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2058,6 +2278,11 @@
       <c r="H45" t="b">
         <v>1</v>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2098,6 +2323,11 @@
       <c r="H46" t="b">
         <v>1</v>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2138,6 +2368,11 @@
       <c r="H47" t="b">
         <v>1</v>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2178,6 +2413,11 @@
       <c r="H48" t="b">
         <v>1</v>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2218,6 +2458,11 @@
       <c r="H49" t="b">
         <v>1</v>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2258,6 +2503,11 @@
       <c r="H50" t="b">
         <v>1</v>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2298,6 +2548,11 @@
       <c r="H51" t="b">
         <v>1</v>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2338,6 +2593,11 @@
       <c r="H52" t="b">
         <v>1</v>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2378,6 +2638,11 @@
       <c r="H53" t="b">
         <v>1</v>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2418,6 +2683,11 @@
       <c r="H54" t="b">
         <v>1</v>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2458,6 +2728,11 @@
       <c r="H55" t="b">
         <v>1</v>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2498,6 +2773,11 @@
       <c r="H56" t="b">
         <v>1</v>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2538,6 +2818,11 @@
       <c r="H57" t="b">
         <v>1</v>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2578,6 +2863,11 @@
       <c r="H58" t="b">
         <v>1</v>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2593,6 +2883,11 @@
       <c r="H59" t="b">
         <v>0</v>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2608,6 +2903,11 @@
       <c r="H60" t="b">
         <v>0</v>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Processo não distribuído</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2623,6 +2923,11 @@
       <c r="H61" t="b">
         <v>0</v>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2638,6 +2943,11 @@
       <c r="H62" t="b">
         <v>0</v>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2653,6 +2963,11 @@
       <c r="H63" t="b">
         <v>0</v>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2668,6 +2983,11 @@
       <c r="H64" t="b">
         <v>0</v>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2683,6 +3003,11 @@
       <c r="H65" t="b">
         <v>0</v>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2698,6 +3023,11 @@
       <c r="H66" t="b">
         <v>0</v>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2713,6 +3043,11 @@
       <c r="H67" t="b">
         <v>0</v>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2728,6 +3063,11 @@
       <c r="H68" t="b">
         <v>0</v>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2743,6 +3083,11 @@
       <c r="H69" t="b">
         <v>0</v>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2758,6 +3103,11 @@
       <c r="H70" t="b">
         <v>0</v>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2773,6 +3123,11 @@
       <c r="H71" t="b">
         <v>0</v>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2788,6 +3143,11 @@
       <c r="H72" t="b">
         <v>0</v>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2803,6 +3163,11 @@
       <c r="H73" t="b">
         <v>0</v>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2818,6 +3183,11 @@
       <c r="H74" t="b">
         <v>0</v>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2833,6 +3203,11 @@
       <c r="H75" t="b">
         <v>0</v>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2848,6 +3223,11 @@
       <c r="H76" t="b">
         <v>0</v>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2863,6 +3243,11 @@
       <c r="H77" t="b">
         <v>0</v>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2878,6 +3263,11 @@
       <c r="H78" t="b">
         <v>0</v>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2893,6 +3283,11 @@
       <c r="H79" t="b">
         <v>0</v>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2908,6 +3303,11 @@
       <c r="H80" t="b">
         <v>0</v>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2923,6 +3323,11 @@
       <c r="H81" t="b">
         <v>0</v>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2938,6 +3343,11 @@
       <c r="H82" t="b">
         <v>0</v>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2953,6 +3363,11 @@
       <c r="H83" t="b">
         <v>0</v>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2968,6 +3383,11 @@
       <c r="H84" t="b">
         <v>0</v>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2983,6 +3403,11 @@
       <c r="H85" t="b">
         <v>0</v>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2998,6 +3423,11 @@
       <c r="H86" t="b">
         <v>0</v>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3013,6 +3443,11 @@
       <c r="H87" t="b">
         <v>0</v>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3028,6 +3463,11 @@
       <c r="H88" t="b">
         <v>0</v>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3043,6 +3483,11 @@
       <c r="H89" t="b">
         <v>0</v>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3058,6 +3503,11 @@
       <c r="H90" t="b">
         <v>0</v>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3073,6 +3523,11 @@
       <c r="H91" t="b">
         <v>0</v>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3088,6 +3543,11 @@
       <c r="H92" t="b">
         <v>0</v>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3103,6 +3563,11 @@
       <c r="H93" t="b">
         <v>0</v>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3118,6 +3583,11 @@
       <c r="H94" t="b">
         <v>0</v>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3133,6 +3603,11 @@
       <c r="H95" t="b">
         <v>0</v>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3148,6 +3623,11 @@
       <c r="H96" t="b">
         <v>0</v>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3163,6 +3643,11 @@
       <c r="H97" t="b">
         <v>0</v>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3178,6 +3663,11 @@
       <c r="H98" t="b">
         <v>0</v>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>Ativo</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3192,6 +3682,3011 @@
       </c>
       <c r="H99" t="b">
         <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>00379505820088260068</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H100" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>10000371120208260260</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H101" t="b">
+        <v>1</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>10022464720188260704</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H102" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>10036538620208260100</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Cumprimento</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H103" t="b">
+        <v>1</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>10038131420208260100</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Cumprimento</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H104" t="b">
+        <v>1</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>10041272820188260100</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H105" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>10047849820188260704</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H106" t="b">
+        <v>1</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>10065940920208260100</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H107" t="b">
+        <v>1</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>10085563320218260100</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H108" t="b">
+        <v>1</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>10096713720188260604</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Cumprimento</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H109" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>10109349320208260100</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H110" t="b">
+        <v>1</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>10122141220198260011</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H111" t="b">
+        <v>1</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>10198352120188260100</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H112" t="b">
+        <v>1</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10198895020198260100</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H113" t="b">
+        <v>1</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>10208996120218260100</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H114" t="b">
+        <v>1</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>10213586320218260100</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H115" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>10225122420188260100</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H116" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>10240934020198260100</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H117" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>10245520820208260100</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H118" t="b">
+        <v>1</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>10321972120198260100</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H119" t="b">
+        <v>1</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>10345694320198260002</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H120" t="b">
+        <v>1</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>10360657020208260100</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>10381130220208260100</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H122" t="b">
+        <v>1</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>10391471220208260100</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H123" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>10430237220208260100</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H124" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>10433398520208260100</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H125" t="b">
+        <v>1</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>10442812020208260100</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H126" t="b">
+        <v>1</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>10461779820208260100</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H127" t="b">
+        <v>1</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>10471087220188260100</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H128" t="b">
+        <v>1</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>10483367720218260100</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H129" t="b">
+        <v>1</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>10489551220188260100</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H130" t="b">
+        <v>1</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>10499773720208260100</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H131" t="b">
+        <v>1</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>10515678320198260100</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H132" t="b">
+        <v>1</v>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>10541348720198260100</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H133" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>10558647020188260100</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H134" t="b">
+        <v>1</v>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>10559581820188260100</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H135" t="b">
+        <v>1</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>10563912220188260100</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H136" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>10591935620198260100</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H137" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>10621298820188260100</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Instauracao</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H138" t="b">
+        <v>1</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>10644101720188260100</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H139" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>10662445520188260100</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H140" t="b">
+        <v>1</v>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>10663138720188260100</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H141" t="b">
+        <v>1</v>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>10696380220208260100</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H142" t="b">
+        <v>1</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10731904320188260100</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H143" t="b">
+        <v>1</v>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>10732224820188260100</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H144" t="b">
+        <v>1</v>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>10780550720218260100</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H145" t="b">
+        <v>1</v>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>10833615420218260100</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H146" t="b">
+        <v>1</v>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>10840731520198260100</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H147" t="b">
+        <v>1</v>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>10863945720188260100</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H148" t="b">
+        <v>1</v>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>10878608620188260100</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H149" t="b">
+        <v>1</v>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>10898236120208260100</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H150" t="b">
+        <v>1</v>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>10899798320198260100</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H151" t="b">
+        <v>1</v>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>10900542520198260100</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H152" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>10918727520208260100</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H153" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>10967120220188260100</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H154" t="b">
+        <v>1</v>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>10967467420188260100</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H155" t="b">
+        <v>1</v>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>10970247520188260100</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H156" t="b">
+        <v>1</v>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>10975651120188260100</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Cumprimento</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H157" t="b">
+        <v>1</v>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>10976213920218260100</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H158" t="b">
+        <v>1</v>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>11014064320208260100</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H159" t="b">
+        <v>1</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>11025078620188260100</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H160" t="b">
+        <v>1</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>11059123320188260100</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H161" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>11074071020218260100</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H162" t="b">
+        <v>1</v>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>11088373120208260100</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H163" t="b">
+        <v>1</v>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>11142373120178260100</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H164" t="b">
+        <v>1</v>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>11160188320208260100</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Instauracao</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H165" t="b">
+        <v>1</v>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>11183387720188260100</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H166" t="b">
+        <v>1</v>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>11183838120188260100</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H167" t="b">
+        <v>1</v>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>11212160920178260100</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H168" t="b">
+        <v>1</v>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>11232254120178260100</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H169" t="b">
+        <v>1</v>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>11242542920178260100</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Instauracao</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H170" t="b">
+        <v>1</v>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>11251131120188260100</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H171" t="b">
+        <v>1</v>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>Encerrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>11255346420198260100</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Agravo de Instrumento</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Cautelar</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H172" t="b">
+        <v>1</v>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>Arquivado administrativamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>11258219520178260100</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Anulacao</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H173" t="b">
+        <v>1</v>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>Remetido a Outro Tribunal</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>11303811220198260100</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Apelação Cível</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Compromisso</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Improvido</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="H174" t="b">
+        <v>1</v>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>Julgado</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update relatório no Quarto
</commit_message>
<xml_diff>
--- a/inst/da_cposg_tidy.xlsx
+++ b/inst/da_cposg_tidy.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -952,7 +952,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3702,7 +3702,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4542,7 +4542,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -5902,7 +5902,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Compromisso</t>
+          <t>Convencao</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">

</xml_diff>